<commit_message>
pr2 schematch, spo e.t.c
</commit_message>
<xml_diff>
--- a/misc/Book2.xlsx
+++ b/misc/Book2.xlsx
@@ -459,7 +459,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,28 +498,28 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -527,28 +527,28 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
         <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
       </c>
       <c r="G3" t="s">
         <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="I3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -556,28 +556,28 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="H4" t="s">
         <v>15</v>
       </c>
       <c r="I4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -588,25 +588,25 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
       </c>
       <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>